<commit_message>
adding US09 and US10 for Sprint 2 and Updated XLS
</commit_message>
<xml_diff>
--- a/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
+++ b/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vedadnya_98/Documents/GitHub/CS-555-Agile_Project_Team/Sprint2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parthxparab/Documents/Spring2020/CS555/Project04/CS-555-Agile_Project_Team/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FBDE86-E74C-C54D-B79B-BDC0C6C9BF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090CFFED-F994-1748-965C-BB461D3137B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="257">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -821,6 +819,30 @@
   </si>
   <si>
     <t>14-16</t>
+  </si>
+  <si>
+    <t>US09()</t>
+  </si>
+  <si>
+    <t>US10()</t>
+  </si>
+  <si>
+    <t>551-574</t>
+  </si>
+  <si>
+    <t>526-547</t>
+  </si>
+  <si>
+    <t>test_userstory09()</t>
+  </si>
+  <si>
+    <t>test_userstory10()</t>
+  </si>
+  <si>
+    <t>30-32</t>
+  </si>
+  <si>
+    <t>34-36</t>
   </si>
 </sst>
 </file>
@@ -2225,7 +2247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2358,7 +2380,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2435,7 +2457,7 @@
         <v>182</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2452,7 +2474,7 @@
         <v>182</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2964,7 +2986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
@@ -3235,7 +3257,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:O1"/>
+      <selection activeCell="E2" sqref="E2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3710,13 +3732,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="14" x14ac:dyDescent="0.15">
@@ -3777,19 +3801,40 @@
         <v>182</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F2">
-        <v>120</v>
+        <v>600</v>
+      </c>
+      <c r="G2">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J2" t="s">
         <v>241</v>
       </c>
+      <c r="K2" t="s">
+        <v>249</v>
+      </c>
+      <c r="L2" t="s">
+        <v>251</v>
+      </c>
       <c r="M2" t="s">
         <v>212</v>
+      </c>
+      <c r="N2" t="s">
+        <v>253</v>
+      </c>
+      <c r="O2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
@@ -3803,19 +3848,40 @@
         <v>182</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E3">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F3">
-        <v>120</v>
+        <v>600</v>
+      </c>
+      <c r="G3">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J3" t="s">
         <v>241</v>
       </c>
+      <c r="K3" t="s">
+        <v>250</v>
+      </c>
+      <c r="L3" t="s">
+        <v>252</v>
+      </c>
       <c r="M3" t="s">
         <v>212</v>
+      </c>
+      <c r="N3" t="s">
+        <v>254</v>
+      </c>
+      <c r="O3" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
@@ -4117,7 +4183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B36" sqref="B36:B37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed US05 and 06
</commit_message>
<xml_diff>
--- a/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
+++ b/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanketpatidar/Desktop/CS 555/Github repositories/CS-555-Agile_Project_Team/Sprint2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parthxparab/Documents/Spring2020/CS555/Project04/CS-555-Agile_Project_Team/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54AC861-6126-574D-BAB3-A96D9E0E5B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D229C22-CF8C-CA46-9F48-4AD31BE357DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="27960" windowHeight="15800" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="273">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -869,6 +867,30 @@
   </si>
   <si>
     <t>66-69</t>
+  </si>
+  <si>
+    <t>US09()</t>
+  </si>
+  <si>
+    <t>US10()</t>
+  </si>
+  <si>
+    <t>667-692</t>
+  </si>
+  <si>
+    <t>636-661</t>
+  </si>
+  <si>
+    <t>test_userstory09()</t>
+  </si>
+  <si>
+    <t>test_userstory10()</t>
+  </si>
+  <si>
+    <t>38-41</t>
+  </si>
+  <si>
+    <t>43-46</t>
   </si>
 </sst>
 </file>
@@ -2405,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2483,7 +2505,7 @@
         <v>182</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2500,7 +2522,7 @@
         <v>182</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -3012,7 +3034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
@@ -3758,8 +3780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3827,7 +3849,7 @@
         <v>182</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E2">
         <v>60</v>
@@ -3835,11 +3857,32 @@
       <c r="F2">
         <v>120</v>
       </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>206</v>
+      </c>
       <c r="J2" t="s">
         <v>241</v>
       </c>
+      <c r="K2" t="s">
+        <v>265</v>
+      </c>
+      <c r="L2" t="s">
+        <v>267</v>
+      </c>
       <c r="M2" t="s">
         <v>212</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
@@ -3853,7 +3896,7 @@
         <v>182</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E3">
         <v>60</v>
@@ -3861,11 +3904,32 @@
       <c r="F3">
         <v>120</v>
       </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>206</v>
+      </c>
       <c r="J3" t="s">
         <v>241</v>
       </c>
+      <c r="K3" t="s">
+        <v>266</v>
+      </c>
+      <c r="L3" t="s">
+        <v>268</v>
+      </c>
       <c r="M3" t="s">
         <v>212</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
added sprint 2 details
</commit_message>
<xml_diff>
--- a/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
+++ b/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parthxparab/Documents/Spring2020/CS555/Project04/CS-555-Agile_Project_Team/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D229C22-CF8C-CA46-9F48-4AD31BE357DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CF732A-A96A-464E-B4EB-D98D7F57D418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="277">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -891,6 +891,18 @@
   </si>
   <si>
     <t>43-46</t>
+  </si>
+  <si>
+    <t>Communicating and discussing progress, practising pair programming</t>
+  </si>
+  <si>
+    <t>Starting project late</t>
+  </si>
+  <si>
+    <t>Communicating and discussing progress, practising pair programming and understanding concepts more clearly</t>
+  </si>
+  <si>
+    <t>Starting project late, Take more time to complete User stories</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1096,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1138,6 +1150,7 @@
     <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2295,7 +2308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2427,7 +2440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -3305,14 +3318,14 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:O1"/>
+      <selection activeCell="A14" sqref="A14:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" customWidth="1"/>
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" customWidth="1"/>
@@ -3759,14 +3772,20 @@
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="67" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="C16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="14" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3778,15 +3797,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" customWidth="1"/>
   </cols>
@@ -4212,6 +4232,39 @@
       </c>
       <c r="O9" s="23" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="B20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -4223,13 +4276,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -4258,6 +4315,166 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated burndown chart Sprint2
</commit_message>
<xml_diff>
--- a/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
+++ b/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parthxparab/Documents/Spring2020/CS555/Project04/CS-555-Agile_Project_Team/Sprint2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranavnair/Desktop/CS-555-Agile_Project_Team/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CF732A-A96A-464E-B4EB-D98D7F57D418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F298116-B22D-EC46-9534-B12793029B13}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="277">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1394,31 +1394,39 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
-                <c:ptCount val="6"/>
+            <c:strRef>
+              <c:f>Burndown!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>42411</c:v>
+                  <c:v>Sprint 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42423</c:v>
+                  <c:v>Sprint 2</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Burndown!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>42415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>42429</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42450</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1443,23 +1451,24 @@
         <c:axId val="1158123744"/>
         <c:axId val="1158126064"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="1158123744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1158126064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1158126064"/>
         <c:scaling>
@@ -1468,7 +1477,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3048,7 +3057,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+      <selection activeCell="A15" sqref="A15:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3239,10 +3248,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3254,55 +3263,101 @@
     <col min="6" max="6" width="14.33203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="32">
-        <v>42411</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="32">
+        <v>42415</v>
+      </c>
+      <c r="C2">
         <v>32</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
-        <v>42423</v>
-      </c>
-      <c r="B3">
+      <c r="F2"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="2">
+        <v>42429</v>
+      </c>
+      <c r="C3">
         <v>24</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>8</v>
       </c>
-      <c r="D3">
-        <v>238</v>
-      </c>
       <c r="E3">
-        <v>280</v>
-      </c>
-      <c r="F3" s="9">
-        <v>50.96</v>
+        <v>523</v>
+      </c>
+      <c r="F3">
+        <v>240</v>
+      </c>
+      <c r="G3" s="9">
+        <f>(E3-E2)/F3*60</f>
+        <v>130.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="7">
+        <v>42450</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>785</v>
+      </c>
+      <c r="F4" s="9">
+        <v>200</v>
+      </c>
+      <c r="G4" s="9">
+        <f>(E4-E3)/F4*60</f>
+        <v>78.600000000000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3317,8 +3372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F20"/>
+    <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3799,8 +3854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4288,7 +4343,7 @@
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
added US 11 & 12
</commit_message>
<xml_diff>
--- a/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
+++ b/Sprint2/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parthxparab/Documents/Spring2020/CS555/Project04/CS-555-Agile_Project_Team/Sprint2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vedadnya_98/Documents/GitHub/CS-555-Agile_Project_Team/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EF29B7-31CE-324E-B09B-061AEF9ADBA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A29B4F-25EA-E449-BAA7-6D0AE1A5B48C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15800" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="289">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -917,6 +919,30 @@
   <si>
     <t>Communicating and discussing progress, 
 practising pair programming and understanding concepts more clearly</t>
+  </si>
+  <si>
+    <t>us34()</t>
+  </si>
+  <si>
+    <t>us20()</t>
+  </si>
+  <si>
+    <t>294-306</t>
+  </si>
+  <si>
+    <t>315-343</t>
+  </si>
+  <si>
+    <t>test_userstory34()</t>
+  </si>
+  <si>
+    <t>test_userstory20()</t>
+  </si>
+  <si>
+    <t>36-40</t>
+  </si>
+  <si>
+    <t>28-34</t>
   </si>
 </sst>
 </file>
@@ -1539,6 +1565,9 @@
                 <c:pt idx="2">
                   <c:v>42444</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>42463</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1556,6 +1585,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3186,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A9" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3576,16 +3608,16 @@
         <v>163</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>84</v>
+        <v>145</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>186</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -3602,7 +3634,7 @@
         <v>186</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -3987,8 +4019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4090,6 +4122,18 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>277</v>
+      </c>
+      <c r="B5" s="13">
+        <v>42463</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>871</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -4592,7 +4636,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="O1" sqref="J1:O1"/>
+      <selection activeCell="G6" sqref="G6:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5082,8 +5126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5222,22 +5266,49 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>84</v>
+        <v>145</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>186</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E6">
         <v>40</v>
       </c>
       <c r="F6">
         <v>100</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J6" t="s">
+        <v>241</v>
+      </c>
+      <c r="K6" t="s">
+        <v>281</v>
+      </c>
+      <c r="L6" t="s">
+        <v>283</v>
+      </c>
+      <c r="M6" t="s">
+        <v>212</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
@@ -5251,13 +5322,40 @@
         <v>186</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E7">
         <v>40</v>
       </c>
       <c r="F7">
         <v>100</v>
+      </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J7" t="s">
+        <v>241</v>
+      </c>
+      <c r="K7" t="s">
+        <v>282</v>
+      </c>
+      <c r="L7" t="s">
+        <v>284</v>
+      </c>
+      <c r="M7" t="s">
+        <v>212</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
@@ -5355,8 +5453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>